<commit_message>
TODC grade norms through rws
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODC_final_gr1_12_10.28.21_fornorms/bln_sum-raw-ss-lookup-tabbed-grade.xlsx
+++ b/OUTPUT-FILES/NORMS/TODC_final_gr1_12_10.28.21_fornorms/bln_sum-raw-ss-lookup-tabbed-grade.xlsx
@@ -7,32 +7,30 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="K-Fall" sheetId="1" r:id="rId1"/>
-    <sheet name="K-Spring" sheetId="2" r:id="rId2"/>
-    <sheet name="1-Fall" sheetId="3" r:id="rId3"/>
-    <sheet name="1-Spring" sheetId="4" r:id="rId4"/>
-    <sheet name="2-Fall" sheetId="5" r:id="rId5"/>
-    <sheet name="2-Spring" sheetId="6" r:id="rId6"/>
-    <sheet name="3-Fall" sheetId="7" r:id="rId7"/>
-    <sheet name="3-Spring" sheetId="8" r:id="rId8"/>
-    <sheet name="4-Fall" sheetId="9" r:id="rId9"/>
-    <sheet name="4-Spring" sheetId="10" r:id="rId10"/>
-    <sheet name="5-Fall" sheetId="11" r:id="rId11"/>
-    <sheet name="5-Spring" sheetId="12" r:id="rId12"/>
-    <sheet name="6-Fall" sheetId="13" r:id="rId13"/>
-    <sheet name="6-Spring" sheetId="14" r:id="rId14"/>
-    <sheet name="7-Fall" sheetId="15" r:id="rId15"/>
-    <sheet name="7-Spring" sheetId="16" r:id="rId16"/>
-    <sheet name="8-Fall" sheetId="17" r:id="rId17"/>
-    <sheet name="8-Spring" sheetId="18" r:id="rId18"/>
-    <sheet name="9-Fall" sheetId="19" r:id="rId19"/>
-    <sheet name="9-Spring" sheetId="20" r:id="rId20"/>
-    <sheet name="10-Fall" sheetId="21" r:id="rId21"/>
-    <sheet name="10-Spring" sheetId="22" r:id="rId22"/>
-    <sheet name="11-Fall" sheetId="23" r:id="rId23"/>
-    <sheet name="11-Spring" sheetId="24" r:id="rId24"/>
-    <sheet name="12-Fall" sheetId="25" r:id="rId25"/>
-    <sheet name="12-Spring" sheetId="26" r:id="rId26"/>
+    <sheet name="1-Fall" sheetId="1" r:id="rId1"/>
+    <sheet name="1-Spring" sheetId="2" r:id="rId2"/>
+    <sheet name="2-Fall" sheetId="3" r:id="rId3"/>
+    <sheet name="2-Spring" sheetId="4" r:id="rId4"/>
+    <sheet name="3-Fall" sheetId="5" r:id="rId5"/>
+    <sheet name="3-Spring" sheetId="6" r:id="rId6"/>
+    <sheet name="4-Fall" sheetId="7" r:id="rId7"/>
+    <sheet name="4-Spring" sheetId="8" r:id="rId8"/>
+    <sheet name="5-Fall" sheetId="9" r:id="rId9"/>
+    <sheet name="5-Spring" sheetId="10" r:id="rId10"/>
+    <sheet name="6-Fall" sheetId="11" r:id="rId11"/>
+    <sheet name="6-Spring" sheetId="12" r:id="rId12"/>
+    <sheet name="7-Fall" sheetId="13" r:id="rId13"/>
+    <sheet name="7-Spring" sheetId="14" r:id="rId14"/>
+    <sheet name="8-Fall" sheetId="15" r:id="rId15"/>
+    <sheet name="8-Spring" sheetId="16" r:id="rId16"/>
+    <sheet name="9-Fall" sheetId="17" r:id="rId17"/>
+    <sheet name="9-Spring" sheetId="18" r:id="rId18"/>
+    <sheet name="10-Fall" sheetId="19" r:id="rId19"/>
+    <sheet name="10-Spring" sheetId="20" r:id="rId20"/>
+    <sheet name="11-Fall" sheetId="21" r:id="rId21"/>
+    <sheet name="11-Spring" sheetId="22" r:id="rId22"/>
+    <sheet name="12-Fall" sheetId="23" r:id="rId23"/>
+    <sheet name="12-Spring" sheetId="24" r:id="rId24"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -463,7 +461,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11">
@@ -471,7 +469,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12">
@@ -479,7 +477,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13">
@@ -487,7 +485,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14">
@@ -495,7 +493,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15">
@@ -503,7 +501,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16">
@@ -511,7 +509,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17">
@@ -519,7 +517,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18">
@@ -527,7 +525,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19">
@@ -535,7 +533,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20">
@@ -543,7 +541,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21">
@@ -551,7 +549,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22">
@@ -559,7 +557,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23">
@@ -567,7 +565,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24">
@@ -575,7 +573,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25">
@@ -720,7 +718,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -728,7 +726,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12">
@@ -736,7 +734,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
@@ -744,7 +742,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14">
@@ -752,7 +750,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15">
@@ -760,7 +758,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16">
@@ -768,7 +766,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17">
@@ -776,7 +774,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18">
@@ -784,7 +782,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19">
@@ -792,7 +790,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20">
@@ -800,7 +798,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21">
@@ -808,7 +806,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22">
@@ -816,7 +814,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23">
@@ -824,7 +822,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24">
@@ -832,7 +830,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25">
@@ -840,7 +838,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26">
@@ -848,7 +846,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27">
@@ -856,7 +854,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28">
@@ -985,7 +983,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12">
@@ -993,7 +991,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
@@ -1001,7 +999,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
@@ -1009,7 +1007,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
@@ -1017,7 +1015,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16">
@@ -1025,7 +1023,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17">
@@ -1033,7 +1031,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18">
@@ -1041,7 +1039,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19">
@@ -1049,7 +1047,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20">
@@ -1057,7 +1055,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21">
@@ -1065,7 +1063,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22">
@@ -1073,7 +1071,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23">
@@ -1081,7 +1079,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24">
@@ -1089,7 +1087,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25">
@@ -1097,7 +1095,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26">
@@ -1105,7 +1103,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27">
@@ -1113,7 +1111,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28">
@@ -1121,7 +1119,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29">
@@ -1242,7 +1240,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
@@ -1250,7 +1248,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13">
@@ -1258,7 +1256,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14">
@@ -1266,7 +1264,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
@@ -1274,7 +1272,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
@@ -1282,7 +1280,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17">
@@ -1290,7 +1288,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18">
@@ -1298,7 +1296,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19">
@@ -1306,7 +1304,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20">
@@ -1314,7 +1312,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21">
@@ -1322,7 +1320,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22">
@@ -1330,7 +1328,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23">
@@ -1338,7 +1336,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24">
@@ -1346,7 +1344,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25">
@@ -1354,7 +1352,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26">
@@ -1362,7 +1360,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27">
@@ -1370,7 +1368,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28">
@@ -1378,7 +1376,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29">
@@ -1499,7 +1497,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
@@ -1507,7 +1505,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13">
@@ -1515,7 +1513,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14">
@@ -1523,7 +1521,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15">
@@ -1531,7 +1529,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16">
@@ -1539,7 +1537,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17">
@@ -1547,7 +1545,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18">
@@ -1555,7 +1553,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19">
@@ -1563,7 +1561,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20">
@@ -1571,7 +1569,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21">
@@ -1579,7 +1577,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22">
@@ -1587,7 +1585,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23">
@@ -1595,7 +1593,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24">
@@ -1603,7 +1601,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25">
@@ -1611,7 +1609,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26">
@@ -1619,7 +1617,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27">
@@ -1627,7 +1625,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28">
@@ -1635,7 +1633,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29">
@@ -1756,7 +1754,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12">
@@ -1764,7 +1762,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13">
@@ -1772,7 +1770,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14">
@@ -1780,7 +1778,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15">
@@ -1788,7 +1786,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16">
@@ -1796,7 +1794,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17">
@@ -1804,7 +1802,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18">
@@ -1812,7 +1810,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19">
@@ -1820,7 +1818,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20">
@@ -1828,7 +1826,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21">
@@ -1836,7 +1834,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22">
@@ -1844,7 +1842,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23">
@@ -1852,7 +1850,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24">
@@ -1860,7 +1858,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25">
@@ -1868,7 +1866,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26">
@@ -1876,7 +1874,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27">
@@ -1884,7 +1882,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28">
@@ -1892,7 +1890,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29">
@@ -1900,7 +1898,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30">
@@ -2013,7 +2011,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12">
@@ -2021,7 +2019,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
@@ -2029,7 +2027,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14">
@@ -2037,7 +2035,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
@@ -2045,7 +2043,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16">
@@ -2053,7 +2051,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
@@ -2061,7 +2059,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18">
@@ -2069,7 +2067,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19">
@@ -2077,7 +2075,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20">
@@ -2085,7 +2083,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21">
@@ -2093,7 +2091,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22">
@@ -2101,7 +2099,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23">
@@ -2109,7 +2107,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24">
@@ -2117,7 +2115,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25">
@@ -2125,7 +2123,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26">
@@ -2133,7 +2131,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27">
@@ -2141,7 +2139,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28">
@@ -2149,7 +2147,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29">
@@ -2157,7 +2155,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30">
@@ -2278,7 +2276,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
@@ -2286,7 +2284,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
@@ -2294,7 +2292,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
@@ -2302,7 +2300,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16">
@@ -2310,7 +2308,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17">
@@ -2318,7 +2316,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
@@ -2326,7 +2324,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19">
@@ -2334,7 +2332,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20">
@@ -2342,7 +2340,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
@@ -2350,7 +2348,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22">
@@ -2358,7 +2356,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23">
@@ -2366,7 +2364,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24">
@@ -2374,7 +2372,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25">
@@ -2382,7 +2380,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26">
@@ -2390,7 +2388,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27">
@@ -2398,7 +2396,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28">
@@ -2406,7 +2404,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29">
@@ -2414,7 +2412,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30">
@@ -2543,7 +2541,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
@@ -2551,7 +2549,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
@@ -2559,7 +2557,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
@@ -2567,7 +2565,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
@@ -2575,7 +2573,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
@@ -2583,7 +2581,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19">
@@ -2591,7 +2589,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20">
@@ -2599,7 +2597,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21">
@@ -2607,7 +2605,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22">
@@ -2615,7 +2613,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23">
@@ -2623,7 +2621,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24">
@@ -2631,7 +2629,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25">
@@ -2639,7 +2637,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26">
@@ -2647,7 +2645,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27">
@@ -2655,7 +2653,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28">
@@ -2663,7 +2661,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29">
@@ -2671,7 +2669,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30">
@@ -2679,7 +2677,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2784,7 +2782,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12">
@@ -2792,7 +2790,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13">
@@ -2800,7 +2798,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
@@ -2808,7 +2806,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
@@ -2816,7 +2814,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16">
@@ -2824,7 +2822,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
@@ -2832,7 +2830,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18">
@@ -2840,7 +2838,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19">
@@ -2848,7 +2846,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20">
@@ -2856,7 +2854,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21">
@@ -2864,7 +2862,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22">
@@ -2872,7 +2870,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23">
@@ -2880,7 +2878,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24">
@@ -2888,7 +2886,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25">
@@ -2896,7 +2894,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26">
@@ -2904,7 +2902,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27">
@@ -2912,7 +2910,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28">
@@ -2920,7 +2918,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29">
@@ -2928,7 +2926,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30">
@@ -2936,7 +2934,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3049,7 +3047,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13">
@@ -3057,7 +3055,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
@@ -3065,7 +3063,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
@@ -3073,7 +3071,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16">
@@ -3081,7 +3079,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
@@ -3089,7 +3087,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
@@ -3097,7 +3095,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19">
@@ -3105,7 +3103,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20">
@@ -3113,7 +3111,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21">
@@ -3121,7 +3119,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22">
@@ -3129,7 +3127,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23">
@@ -3137,7 +3135,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24">
@@ -3145,7 +3143,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25">
@@ -3153,7 +3151,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26">
@@ -3161,7 +3159,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27">
@@ -3169,7 +3167,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28">
@@ -3177,7 +3175,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29">
@@ -3185,7 +3183,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30">
@@ -3193,7 +3191,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3290,7 +3288,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11">
@@ -3298,7 +3296,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -3306,7 +3304,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13">
@@ -3314,7 +3312,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14">
@@ -3322,7 +3320,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15">
@@ -3330,7 +3328,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16">
@@ -3338,7 +3336,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17">
@@ -3346,7 +3344,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18">
@@ -3354,7 +3352,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19">
@@ -3362,7 +3360,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20">
@@ -3370,7 +3368,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21">
@@ -3378,7 +3376,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22">
@@ -3386,7 +3384,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23">
@@ -3394,7 +3392,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24">
@@ -3402,7 +3400,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25">
@@ -3555,7 +3553,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12">
@@ -3579,7 +3577,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
@@ -3587,7 +3585,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16">
@@ -3595,7 +3593,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
@@ -3603,7 +3601,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
@@ -3611,7 +3609,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
@@ -3619,7 +3617,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20">
@@ -3627,7 +3625,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21">
@@ -3635,7 +3633,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22">
@@ -3643,7 +3641,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23">
@@ -3651,7 +3649,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24">
@@ -3659,7 +3657,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25">
@@ -3667,7 +3665,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26">
@@ -3675,7 +3673,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27">
@@ -3683,7 +3681,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28">
@@ -3691,7 +3689,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29">
@@ -3699,7 +3697,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30">
@@ -3707,7 +3705,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3804,7 +3802,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11">
@@ -3844,7 +3842,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16">
@@ -3852,7 +3850,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
@@ -3860,7 +3858,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
@@ -3868,7 +3866,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
@@ -3876,7 +3874,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20">
@@ -3884,7 +3882,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21">
@@ -3892,7 +3890,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22">
@@ -3900,7 +3898,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23">
@@ -3908,7 +3906,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24">
@@ -3916,7 +3914,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25">
@@ -3924,7 +3922,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26">
@@ -3932,7 +3930,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27">
@@ -3940,7 +3938,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28">
@@ -3948,7 +3946,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29">
@@ -3956,7 +3954,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30">
@@ -3964,7 +3962,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4061,7 +4059,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
@@ -4093,7 +4091,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15">
@@ -4109,7 +4107,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
@@ -4117,7 +4115,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
@@ -4125,7 +4123,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19">
@@ -4133,7 +4131,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20">
@@ -4141,7 +4139,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21">
@@ -4149,7 +4147,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22">
@@ -4157,7 +4155,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23">
@@ -4165,7 +4163,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24">
@@ -4173,7 +4171,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25">
@@ -4181,7 +4179,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26">
@@ -4189,7 +4187,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27">
@@ -4197,7 +4195,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28">
@@ -4205,7 +4203,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29">
@@ -4213,7 +4211,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30">
@@ -4221,7 +4219,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -4318,7 +4316,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
@@ -4326,7 +4324,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
@@ -4334,7 +4332,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
@@ -4350,7 +4348,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15">
@@ -4374,7 +4372,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18">
@@ -4382,7 +4380,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19">
@@ -4390,7 +4388,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20">
@@ -4398,7 +4396,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21">
@@ -4406,7 +4404,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22">
@@ -4414,7 +4412,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23">
@@ -4422,7 +4420,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24">
@@ -4430,7 +4428,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25">
@@ -4438,7 +4436,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26">
@@ -4446,7 +4444,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27">
@@ -4454,7 +4452,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28">
@@ -4462,7 +4460,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29">
@@ -4470,7 +4468,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30">
@@ -4478,7 +4476,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -4575,520 +4573,6 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>122</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>raw</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>ss</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>121</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>raw</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>ss</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
         <v>43</v>
       </c>
     </row>
@@ -5346,7 +4830,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11">
@@ -5354,7 +4838,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12">
@@ -5362,7 +4846,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13">
@@ -5370,7 +4854,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14">
@@ -5378,7 +4862,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15">
@@ -5386,7 +4870,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16">
@@ -5394,7 +4878,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17">
@@ -5402,7 +4886,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18">
@@ -5410,7 +4894,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19">
@@ -5418,7 +4902,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20">
@@ -5426,7 +4910,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21">
@@ -5434,7 +4918,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22">
@@ -5442,7 +4926,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23">
@@ -5450,7 +4934,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24">
@@ -5458,7 +4942,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25">
@@ -5466,7 +4950,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26">
@@ -5603,7 +5087,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11">
@@ -5611,7 +5095,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12">
@@ -5619,7 +5103,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13">
@@ -5627,7 +5111,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14">
@@ -5635,7 +5119,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15">
@@ -5643,7 +5127,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16">
@@ -5651,7 +5135,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17">
@@ -5659,7 +5143,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18">
@@ -5667,7 +5151,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19">
@@ -5675,7 +5159,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20">
@@ -5683,7 +5167,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21">
@@ -5691,7 +5175,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22">
@@ -5699,7 +5183,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23">
@@ -5707,7 +5191,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24">
@@ -5715,7 +5199,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25">
@@ -5723,7 +5207,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26">
@@ -5860,7 +5344,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11">
@@ -5868,7 +5352,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
@@ -5876,7 +5360,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13">
@@ -5884,7 +5368,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14">
@@ -5892,7 +5376,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15">
@@ -5900,7 +5384,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16">
@@ -5908,7 +5392,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17">
@@ -5916,7 +5400,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18">
@@ -5924,7 +5408,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19">
@@ -5932,7 +5416,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20">
@@ -5940,7 +5424,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21">
@@ -5948,7 +5432,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22">
@@ -5956,7 +5440,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23">
@@ -5964,7 +5448,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24">
@@ -5972,7 +5456,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25">
@@ -5980,7 +5464,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26">
@@ -6117,7 +5601,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
@@ -6125,7 +5609,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12">
@@ -6133,7 +5617,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13">
@@ -6141,7 +5625,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14">
@@ -6149,7 +5633,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15">
@@ -6157,7 +5641,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16">
@@ -6165,7 +5649,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17">
@@ -6173,7 +5657,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18">
@@ -6181,7 +5665,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19">
@@ -6189,7 +5673,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20">
@@ -6197,7 +5681,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21">
@@ -6205,7 +5689,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22">
@@ -6213,7 +5697,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23">
@@ -6221,7 +5705,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24">
@@ -6229,7 +5713,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25">
@@ -6237,7 +5721,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26">
@@ -6245,7 +5729,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27">
@@ -6374,7 +5858,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
@@ -6382,7 +5866,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12">
@@ -6390,7 +5874,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13">
@@ -6398,7 +5882,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14">
@@ -6406,7 +5890,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15">
@@ -6414,7 +5898,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16">
@@ -6422,7 +5906,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17">
@@ -6430,7 +5914,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18">
@@ -6438,7 +5922,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19">
@@ -6446,7 +5930,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20">
@@ -6454,7 +5938,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21">
@@ -6462,7 +5946,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22">
@@ -6470,7 +5954,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23">
@@ -6478,7 +5962,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24">
@@ -6486,7 +5970,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25">
@@ -6494,7 +5978,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26">
@@ -6502,7 +5986,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27">
@@ -6631,7 +6115,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11">
@@ -6639,7 +6123,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12">
@@ -6647,7 +6131,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13">
@@ -6655,7 +6139,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14">
@@ -6663,7 +6147,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15">
@@ -6671,7 +6155,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16">
@@ -6679,7 +6163,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17">
@@ -6687,7 +6171,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18">
@@ -6695,7 +6179,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19">
@@ -6703,7 +6187,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20">
@@ -6711,7 +6195,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21">
@@ -6719,7 +6203,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22">
@@ -6727,7 +6211,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23">
@@ -6735,7 +6219,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24">
@@ -6743,7 +6227,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25">
@@ -6751,7 +6235,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26">
@@ -6759,7 +6243,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27">
@@ -6767,7 +6251,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28">
@@ -6888,7 +6372,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -6896,7 +6380,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12">
@@ -6904,7 +6388,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13">
@@ -6912,7 +6396,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14">
@@ -6920,7 +6404,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15">
@@ -6928,7 +6412,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16">
@@ -6936,7 +6420,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17">
@@ -6944,7 +6428,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18">
@@ -6952,7 +6436,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19">
@@ -6960,7 +6444,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20">
@@ -6968,7 +6452,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21">
@@ -6976,7 +6460,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22">
@@ -6984,7 +6468,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23">
@@ -6992,7 +6476,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24">
@@ -7000,7 +6484,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25">
@@ -7008,7 +6492,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26">
@@ -7016,7 +6500,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27">
@@ -7024,7 +6508,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28">

</xml_diff>

<commit_message>
TODC grade norms through iwr
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODC_final_gr1_12_10.28.21_fornorms/bln_sum-raw-ss-lookup-tabbed-grade.xlsx
+++ b/OUTPUT-FILES/NORMS/TODC_final_gr1_12_10.28.21_fornorms/bln_sum-raw-ss-lookup-tabbed-grade.xlsx
@@ -445,7 +445,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
@@ -453,7 +453,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -461,7 +461,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -469,7 +469,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>68</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -477,7 +477,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>74</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
@@ -485,7 +485,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14">
@@ -493,7 +493,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15">
@@ -501,7 +501,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16">
@@ -509,7 +509,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17">
@@ -517,7 +517,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18">
@@ -525,7 +525,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19">
@@ -533,7 +533,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20">
@@ -541,7 +541,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21">
@@ -549,7 +549,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22">
@@ -557,7 +557,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23">
@@ -565,7 +565,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24">
@@ -573,7 +573,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25">
@@ -581,7 +581,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26">
@@ -589,7 +589,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27">
@@ -718,7 +718,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -726,7 +726,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -734,7 +734,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -742,7 +742,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13">
@@ -750,7 +750,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
@@ -758,7 +758,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15">
@@ -766,7 +766,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16">
@@ -774,7 +774,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17">
@@ -782,7 +782,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18">
@@ -798,7 +798,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20">
@@ -806,7 +806,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21">
@@ -830,7 +830,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24">
@@ -838,7 +838,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25">
@@ -854,7 +854,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27">
@@ -862,7 +862,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28">
@@ -870,7 +870,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29">
@@ -878,7 +878,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30">
@@ -983,7 +983,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -991,7 +991,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -999,7 +999,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -1007,7 +1007,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13">
@@ -1015,7 +1015,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
@@ -1023,7 +1023,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15">
@@ -1031,7 +1031,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16">
@@ -1039,7 +1039,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
@@ -1047,7 +1047,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
@@ -1055,7 +1055,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19">
@@ -1063,7 +1063,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20">
@@ -1071,7 +1071,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21">
@@ -1079,7 +1079,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22">
@@ -1087,7 +1087,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23">
@@ -1095,7 +1095,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24">
@@ -1103,7 +1103,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25">
@@ -1111,7 +1111,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26">
@@ -1119,7 +1119,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27">
@@ -1127,7 +1127,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28">
@@ -1135,7 +1135,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29">
@@ -1143,7 +1143,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30">
@@ -1256,7 +1256,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -1264,7 +1264,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -1272,7 +1272,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13">
@@ -1280,7 +1280,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
@@ -1288,7 +1288,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -1296,7 +1296,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16">
@@ -1304,7 +1304,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
@@ -1312,7 +1312,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18">
@@ -1320,7 +1320,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19">
@@ -1328,7 +1328,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20">
@@ -1336,7 +1336,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21">
@@ -1344,7 +1344,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22">
@@ -1352,7 +1352,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23">
@@ -1360,7 +1360,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24">
@@ -1368,7 +1368,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25">
@@ -1376,7 +1376,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26">
@@ -1384,7 +1384,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27">
@@ -1392,7 +1392,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28">
@@ -1400,7 +1400,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29">
@@ -1408,7 +1408,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30">
@@ -1521,7 +1521,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -1529,7 +1529,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -1537,7 +1537,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
@@ -1545,7 +1545,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
@@ -1553,7 +1553,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -1561,7 +1561,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16">
@@ -1569,7 +1569,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
@@ -1577,7 +1577,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
@@ -1585,7 +1585,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19">
@@ -1593,7 +1593,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20">
@@ -1601,7 +1601,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21">
@@ -1609,7 +1609,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22">
@@ -1617,7 +1617,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23">
@@ -1625,7 +1625,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24">
@@ -1633,7 +1633,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25">
@@ -1641,7 +1641,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26">
@@ -1649,7 +1649,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27">
@@ -1657,7 +1657,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28">
@@ -1665,7 +1665,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29">
@@ -1673,7 +1673,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30">
@@ -1681,7 +1681,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31">
@@ -1786,7 +1786,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -1794,7 +1794,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -1802,7 +1802,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13">
@@ -1810,7 +1810,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
@@ -1818,7 +1818,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -1826,7 +1826,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16">
@@ -1834,7 +1834,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
@@ -1842,7 +1842,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
@@ -1850,7 +1850,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19">
@@ -1858,7 +1858,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20">
@@ -1866,7 +1866,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21">
@@ -1874,7 +1874,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22">
@@ -1882,7 +1882,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23">
@@ -1890,7 +1890,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24">
@@ -1898,7 +1898,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25">
@@ -1906,7 +1906,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26">
@@ -1914,7 +1914,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27">
@@ -1922,7 +1922,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28">
@@ -1930,7 +1930,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29">
@@ -1938,7 +1938,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30">
@@ -1946,7 +1946,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31">
@@ -2051,7 +2051,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -2059,7 +2059,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -2067,7 +2067,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13">
@@ -2075,7 +2075,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
@@ -2083,7 +2083,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15">
@@ -2091,7 +2091,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16">
@@ -2099,7 +2099,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17">
@@ -2115,7 +2115,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
@@ -2123,7 +2123,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20">
@@ -2131,7 +2131,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21">
@@ -2139,7 +2139,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22">
@@ -2147,7 +2147,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23">
@@ -2155,7 +2155,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24">
@@ -2163,7 +2163,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25">
@@ -2171,7 +2171,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26">
@@ -2179,7 +2179,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27">
@@ -2187,7 +2187,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28">
@@ -2195,7 +2195,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29">
@@ -2203,7 +2203,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30">
@@ -2316,7 +2316,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -2324,7 +2324,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -2332,7 +2332,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
@@ -2340,7 +2340,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
@@ -2348,7 +2348,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15">
@@ -2364,7 +2364,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17">
@@ -2412,7 +2412,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23">
@@ -2420,7 +2420,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24">
@@ -2428,7 +2428,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25">
@@ -2436,7 +2436,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26">
@@ -2444,7 +2444,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27">
@@ -2452,7 +2452,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28">
@@ -2460,7 +2460,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29">
@@ -2468,7 +2468,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30">
@@ -2484,7 +2484,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2581,7 +2581,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -2589,7 +2589,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -2597,7 +2597,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
@@ -2613,7 +2613,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -2621,7 +2621,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16">
@@ -2629,7 +2629,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17">
@@ -2637,7 +2637,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18">
@@ -2645,7 +2645,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19">
@@ -2677,7 +2677,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23">
@@ -2693,7 +2693,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25">
@@ -2701,7 +2701,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26">
@@ -2709,7 +2709,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27">
@@ -2717,7 +2717,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28">
@@ -2725,7 +2725,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29">
@@ -2749,7 +2749,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2854,7 +2854,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -2862,7 +2862,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13">
@@ -2870,7 +2870,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14">
@@ -2878,7 +2878,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -2886,7 +2886,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16">
@@ -2894,7 +2894,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17">
@@ -2902,7 +2902,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -2910,7 +2910,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
@@ -2918,7 +2918,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20">
@@ -2926,7 +2926,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
@@ -2934,7 +2934,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22">
@@ -2966,7 +2966,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26">
@@ -2974,7 +2974,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27">
@@ -2982,7 +2982,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28">
@@ -3006,7 +3006,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31">
@@ -3014,7 +3014,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3119,7 +3119,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12">
@@ -3127,7 +3127,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13">
@@ -3135,7 +3135,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14">
@@ -3143,7 +3143,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -3151,7 +3151,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16">
@@ -3159,7 +3159,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17">
@@ -3167,7 +3167,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -3175,7 +3175,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
@@ -3183,7 +3183,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
@@ -3191,7 +3191,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
@@ -3199,7 +3199,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22">
@@ -3215,7 +3215,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24">
@@ -3231,7 +3231,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26">
@@ -3271,7 +3271,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31">
@@ -3279,7 +3279,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3360,7 +3360,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
@@ -3368,7 +3368,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -3376,7 +3376,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -3384,7 +3384,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -3392,7 +3392,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>70</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13">
@@ -3400,7 +3400,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
@@ -3408,7 +3408,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
@@ -3416,7 +3416,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16">
@@ -3424,7 +3424,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17">
@@ -3432,7 +3432,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18">
@@ -3440,7 +3440,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19">
@@ -3448,7 +3448,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20">
@@ -3456,7 +3456,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21">
@@ -3464,7 +3464,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22">
@@ -3472,7 +3472,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23">
@@ -3480,7 +3480,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24">
@@ -3488,7 +3488,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25">
@@ -3496,7 +3496,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26">
@@ -3504,7 +3504,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27">
@@ -3657,7 +3657,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13">
@@ -3665,7 +3665,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14">
@@ -3673,7 +3673,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -3681,7 +3681,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16">
@@ -3689,7 +3689,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17">
@@ -3697,7 +3697,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -3705,7 +3705,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19">
@@ -3713,7 +3713,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
@@ -3721,7 +3721,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21">
@@ -3729,7 +3729,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22">
@@ -3737,7 +3737,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23">
@@ -3745,7 +3745,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24">
@@ -3801,7 +3801,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31">
@@ -3809,7 +3809,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3914,7 +3914,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12">
@@ -3922,7 +3922,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13">
@@ -3930,7 +3930,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
@@ -3938,7 +3938,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15">
@@ -3946,7 +3946,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16">
@@ -3954,7 +3954,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17">
@@ -3962,7 +3962,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -3970,7 +3970,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19">
@@ -3978,7 +3978,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
@@ -3986,7 +3986,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21">
@@ -3994,7 +3994,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22">
@@ -4002,7 +4002,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23">
@@ -4010,7 +4010,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24">
@@ -4066,7 +4066,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31">
@@ -4074,7 +4074,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4179,7 +4179,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12">
@@ -4187,7 +4187,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13">
@@ -4195,7 +4195,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14">
@@ -4203,7 +4203,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15">
@@ -4211,7 +4211,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16">
@@ -4219,7 +4219,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17">
@@ -4227,7 +4227,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -4235,7 +4235,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19">
@@ -4243,7 +4243,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
@@ -4251,7 +4251,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21">
@@ -4259,7 +4259,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22">
@@ -4267,7 +4267,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23">
@@ -4275,7 +4275,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24">
@@ -4299,7 +4299,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27">
@@ -4307,7 +4307,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28">
@@ -4331,7 +4331,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31">
@@ -4339,7 +4339,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4436,7 +4436,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
@@ -4444,7 +4444,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
@@ -4452,7 +4452,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
@@ -4460,7 +4460,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
@@ -4468,7 +4468,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15">
@@ -4476,7 +4476,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16">
@@ -4484,7 +4484,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17">
@@ -4492,7 +4492,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -4500,7 +4500,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19">
@@ -4508,7 +4508,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
@@ -4516,7 +4516,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21">
@@ -4524,7 +4524,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22">
@@ -4532,7 +4532,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23">
@@ -4548,7 +4548,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25">
@@ -4556,7 +4556,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26">
@@ -4564,7 +4564,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27">
@@ -4572,7 +4572,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28">
@@ -4580,7 +4580,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29">
@@ -4588,7 +4588,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30">
@@ -4604,7 +4604,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4701,7 +4701,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11">
@@ -4709,7 +4709,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12">
@@ -4717,7 +4717,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13">
@@ -4725,7 +4725,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
@@ -4733,7 +4733,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
@@ -4741,7 +4741,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16">
@@ -4749,7 +4749,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17">
@@ -4757,7 +4757,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -4765,7 +4765,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
@@ -4773,7 +4773,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
@@ -4781,7 +4781,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21">
@@ -4797,7 +4797,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23">
@@ -4805,7 +4805,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24">
@@ -4813,7 +4813,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25">
@@ -4821,7 +4821,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26">
@@ -4829,7 +4829,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27">
@@ -4837,7 +4837,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28">
@@ -4845,7 +4845,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29">
@@ -4853,7 +4853,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30">
@@ -4861,7 +4861,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31">
@@ -4958,7 +4958,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -4966,7 +4966,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -4974,7 +4974,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -4982,7 +4982,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13">
@@ -4990,7 +4990,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
@@ -4998,7 +4998,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
@@ -5006,7 +5006,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16">
@@ -5014,7 +5014,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17">
@@ -5022,7 +5022,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18">
@@ -5038,7 +5038,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20">
@@ -5070,7 +5070,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24">
@@ -5078,7 +5078,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25">
@@ -5086,7 +5086,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26">
@@ -5094,7 +5094,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27">
@@ -5223,7 +5223,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -5231,7 +5231,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -5239,7 +5239,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -5247,7 +5247,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
@@ -5255,7 +5255,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14">
@@ -5263,7 +5263,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15">
@@ -5271,7 +5271,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16">
@@ -5295,7 +5295,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19">
@@ -5303,7 +5303,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20">
@@ -5311,7 +5311,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21">
@@ -5319,7 +5319,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22">
@@ -5327,7 +5327,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23">
@@ -5359,7 +5359,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27">
@@ -5367,7 +5367,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28">
@@ -5488,7 +5488,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -5496,7 +5496,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -5504,7 +5504,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -5512,7 +5512,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
@@ -5520,7 +5520,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14">
@@ -5528,7 +5528,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15">
@@ -5536,7 +5536,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16">
@@ -5544,7 +5544,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17">
@@ -5552,7 +5552,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18">
@@ -5560,7 +5560,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19">
@@ -5568,7 +5568,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20">
@@ -5576,7 +5576,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21">
@@ -5584,7 +5584,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22">
@@ -5592,7 +5592,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23">
@@ -5600,7 +5600,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24">
@@ -5608,7 +5608,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25">
@@ -5616,7 +5616,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26">
@@ -5632,7 +5632,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28">
@@ -5753,7 +5753,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -5761,7 +5761,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -5769,7 +5769,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -5777,7 +5777,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13">
@@ -5785,7 +5785,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
@@ -5793,7 +5793,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
@@ -5801,7 +5801,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
@@ -5817,7 +5817,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18">
@@ -5825,7 +5825,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19">
@@ -5833,7 +5833,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20">
@@ -5841,7 +5841,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21">
@@ -5849,7 +5849,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22">
@@ -5857,7 +5857,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23">
@@ -5865,7 +5865,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24">
@@ -5873,7 +5873,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25">
@@ -5881,7 +5881,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26">
@@ -6018,7 +6018,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -6026,7 +6026,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -6034,7 +6034,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -6042,7 +6042,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13">
@@ -6050,7 +6050,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14">
@@ -6058,7 +6058,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
@@ -6066,7 +6066,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16">
@@ -6082,7 +6082,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18">
@@ -6090,7 +6090,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19">
@@ -6098,7 +6098,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20">
@@ -6106,7 +6106,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21">
@@ -6114,7 +6114,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22">
@@ -6122,7 +6122,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23">
@@ -6130,7 +6130,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24">
@@ -6138,7 +6138,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25">
@@ -6146,7 +6146,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26">
@@ -6283,7 +6283,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -6291,7 +6291,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -6299,7 +6299,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -6307,7 +6307,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13">
@@ -6315,7 +6315,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14">
@@ -6323,7 +6323,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
@@ -6331,7 +6331,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16">
@@ -6339,7 +6339,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17">
@@ -6363,7 +6363,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20">
@@ -6371,7 +6371,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21">
@@ -6379,7 +6379,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22">
@@ -6387,7 +6387,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23">
@@ -6395,7 +6395,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24">
@@ -6403,7 +6403,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25">
@@ -6435,7 +6435,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29">
@@ -6548,7 +6548,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -6556,7 +6556,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -6564,7 +6564,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -6572,7 +6572,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13">
@@ -6580,7 +6580,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14">
@@ -6588,7 +6588,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15">
@@ -6596,7 +6596,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
@@ -6604,7 +6604,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
@@ -6612,7 +6612,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18">
@@ -6628,7 +6628,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20">
@@ -6668,7 +6668,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25">
@@ -6700,7 +6700,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29">

</xml_diff>